<commit_message>
Progresso no sistema de jogar
</commit_message>
<xml_diff>
--- a/campo.xlsx
+++ b/campo.xlsx
@@ -2,13 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="config" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="jogo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="jogo1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="jogo2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="jogo3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="jogo4" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,13 +22,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -35,7 +51,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -45,13 +68,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -130,10 +168,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -171,69 +209,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -257,54 +297,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -314,7 +353,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -323,7 +362,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -332,7 +371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -340,10 +379,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -372,7 +411,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -385,13 +424,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -411,7 +449,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
@@ -422,14 +460,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B3"/>
@@ -439,40 +477,555 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Linhas</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>Colunas</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>dificuldade</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="14.14785714285714" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E1" s="5" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Linhas</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>-1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Colunas</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dificuldade</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>